<commit_message>
add nxTON for DCM period stretching
</commit_message>
<xml_diff>
--- a/data/ic_params.xlsx
+++ b/data/ic_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://renesasgroup-my.sharepoint.com/personal/gary_kidwell_wz_renesas_com/Documents/python/charger/mathmodels/3lvlbuck/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://renesasgroup-my.sharepoint.com/personal/gary_kidwell_wz_renesas_com/Documents/python/charger/mathmodels/pdis_2or3lvl_bb/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="113" documentId="8_{F84FD8E5-1FFF-4787-86AE-DA4064EEAF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D85585C-A945-49AB-B4E4-20090BE0EC2D}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="5205" windowWidth="20970" windowHeight="15150" xr2:uid="{CD76860F-921B-4D74-8C7E-AD0F0543B9C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16260" xr2:uid="{CD76860F-921B-4D74-8C7E-AD0F0543B9C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -197,9 +197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -237,7 +237,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -343,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,7 +485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,7 +496,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add ihlp, transpose mosfet_data
</commit_message>
<xml_diff>
--- a/data/ic_params.xlsx
+++ b/data/ic_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://renesasgroup-my.sharepoint.com/personal/gary_kidwell_wz_renesas_com/Documents/python/charger/mathmodels/pdis_2or3lvl_bb/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="8_{F84FD8E5-1FFF-4787-86AE-DA4064EEAF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D85585C-A945-49AB-B4E4-20090BE0EC2D}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{F84FD8E5-1FFF-4787-86AE-DA4064EEAF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AE42C3B-AF47-404E-8EFE-3E74FAB6841D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16260" xr2:uid="{CD76860F-921B-4D74-8C7E-AD0F0543B9C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{CD76860F-921B-4D74-8C7E-AD0F0543B9C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +682,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F9">
         <v>10</v>

</xml_diff>